<commit_message>
change in test data
</commit_message>
<xml_diff>
--- a/testdata/testdata.xlsx
+++ b/testdata/testdata.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -73,9 +72,6 @@
     <t>createtask_ID</t>
   </si>
   <si>
-    <t>testing</t>
-  </si>
-  <si>
     <t>Billable</t>
   </si>
   <si>
@@ -95,6 +91,9 @@
   </si>
   <si>
     <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -475,7 +474,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,19 +643,19 @@
         <v>15</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="G8" s="5">
         <v>43527</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -673,42 +672,42 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -719,7 +718,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>

</xml_diff>